<commit_message>
:pencil: added 2013 data
</commit_message>
<xml_diff>
--- a/data/raw/raw_inss.xlsx
+++ b/data/raw/raw_inss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\inss_nicaragua\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514D0E86-2F4A-4701-B6D1-16FE37D6EE71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD84263-7627-4B8D-B279-055858B388A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{ACF5B5E4-8843-4660-869C-325022BB6AF5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="29">
   <si>
     <t>Hombres</t>
   </si>
@@ -118,42 +118,6 @@
   </si>
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>0-15</t>
-  </si>
-  <si>
-    <t>15-20</t>
-  </si>
-  <si>
-    <t>20-25</t>
-  </si>
-  <si>
-    <t>25-30</t>
-  </si>
-  <si>
-    <t>30-35</t>
-  </si>
-  <si>
-    <t>35-40</t>
-  </si>
-  <si>
-    <t>40-45</t>
-  </si>
-  <si>
-    <t>45-50</t>
-  </si>
-  <si>
-    <t>50-55</t>
-  </si>
-  <si>
-    <t>55-60</t>
-  </si>
-  <si>
-    <t>60-65</t>
-  </si>
-  <si>
-    <t>66 y Más</t>
   </si>
   <si>
     <t>gender</t>
@@ -516,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DD7A6D-0159-4732-B968-95910A7019B7}">
   <dimension ref="A1:O313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="S276" sqref="S276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +491,7 @@
         <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3961,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D74">
         <v>92</v>
@@ -4008,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D75">
         <v>11472</v>
@@ -4055,7 +4019,7 @@
         <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D76">
         <v>64571</v>
@@ -4102,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D77">
         <v>77851</v>
@@ -4149,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D78">
         <v>75359</v>
@@ -4196,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D79">
         <v>54444</v>
@@ -4243,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D80">
         <v>41322</v>
@@ -4290,7 +4254,7 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D81">
         <v>34486</v>
@@ -4337,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D82">
         <v>28931</v>
@@ -4384,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D83">
         <v>21492</v>
@@ -4431,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D84">
         <v>7451</v>
@@ -4478,7 +4442,7 @@
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D85">
         <v>3989</v>
@@ -4525,7 +4489,7 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D86">
         <v>60</v>
@@ -4572,7 +4536,7 @@
         <v>26</v>
       </c>
       <c r="C87" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D87">
         <v>5574</v>
@@ -4619,7 +4583,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D88">
         <v>40182</v>
@@ -4666,7 +4630,7 @@
         <v>26</v>
       </c>
       <c r="C89" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D89">
         <v>56159</v>
@@ -4713,7 +4677,7 @@
         <v>26</v>
       </c>
       <c r="C90" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D90">
         <v>57582</v>
@@ -4760,7 +4724,7 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D91">
         <v>42080</v>
@@ -4807,7 +4771,7 @@
         <v>26</v>
       </c>
       <c r="C92" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D92">
         <v>34103</v>
@@ -4854,7 +4818,7 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D93">
         <v>30182</v>
@@ -4901,7 +4865,7 @@
         <v>26</v>
       </c>
       <c r="C94" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D94">
         <v>23909</v>
@@ -4948,7 +4912,7 @@
         <v>26</v>
       </c>
       <c r="C95" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D95">
         <v>14864</v>
@@ -4995,7 +4959,7 @@
         <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D96">
         <v>4845</v>
@@ -5042,7 +5006,7 @@
         <v>26</v>
       </c>
       <c r="C97" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D97">
         <v>1885</v>
@@ -5089,7 +5053,7 @@
         <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D98">
         <v>43</v>
@@ -5136,7 +5100,7 @@
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D99">
         <v>12627</v>
@@ -5183,7 +5147,7 @@
         <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D100">
         <v>62337</v>
@@ -5230,7 +5194,7 @@
         <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D101">
         <v>75072</v>
@@ -5277,7 +5241,7 @@
         <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D102">
         <v>70339</v>
@@ -5324,7 +5288,7 @@
         <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D103">
         <v>50713</v>
@@ -5371,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="C104" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D104">
         <v>38227</v>
@@ -5418,7 +5382,7 @@
         <v>0</v>
       </c>
       <c r="C105" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D105">
         <v>32623</v>
@@ -5465,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="C106" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D106">
         <v>26485</v>
@@ -5512,7 +5476,7 @@
         <v>0</v>
       </c>
       <c r="C107" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D107">
         <v>19354</v>
@@ -5559,7 +5523,7 @@
         <v>0</v>
       </c>
       <c r="C108" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D108">
         <v>6720</v>
@@ -5606,7 +5570,7 @@
         <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D109">
         <v>3864</v>
@@ -5653,7 +5617,7 @@
         <v>26</v>
       </c>
       <c r="C110" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D110">
         <v>10</v>
@@ -5700,7 +5664,7 @@
         <v>26</v>
       </c>
       <c r="C111" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D111">
         <v>6062</v>
@@ -5747,7 +5711,7 @@
         <v>26</v>
       </c>
       <c r="C112" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D112">
         <v>39648</v>
@@ -5794,7 +5758,7 @@
         <v>26</v>
       </c>
       <c r="C113" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D113">
         <v>54479</v>
@@ -5841,7 +5805,7 @@
         <v>26</v>
       </c>
       <c r="C114" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D114">
         <v>53446</v>
@@ -5888,7 +5852,7 @@
         <v>26</v>
       </c>
       <c r="C115" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D115">
         <v>39134</v>
@@ -5935,7 +5899,7 @@
         <v>26</v>
       </c>
       <c r="C116" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D116">
         <v>31747</v>
@@ -5982,7 +5946,7 @@
         <v>26</v>
       </c>
       <c r="C117" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D117">
         <v>27943</v>
@@ -6029,7 +5993,7 @@
         <v>26</v>
       </c>
       <c r="C118" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D118">
         <v>21183</v>
@@ -6076,7 +6040,7 @@
         <v>26</v>
       </c>
       <c r="C119" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D119">
         <v>12882</v>
@@ -6123,7 +6087,7 @@
         <v>26</v>
       </c>
       <c r="C120" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D120">
         <v>4233</v>
@@ -6170,7 +6134,7 @@
         <v>26</v>
       </c>
       <c r="C121" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D121">
         <v>1699</v>
@@ -6217,6 +6181,42 @@
         <v>0</v>
       </c>
       <c r="C122" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122">
+        <v>29</v>
+      </c>
+      <c r="E122">
+        <v>34</v>
+      </c>
+      <c r="F122">
+        <v>28</v>
+      </c>
+      <c r="G122">
+        <v>27</v>
+      </c>
+      <c r="H122">
+        <v>20</v>
+      </c>
+      <c r="I122">
+        <v>19</v>
+      </c>
+      <c r="J122">
+        <v>12</v>
+      </c>
+      <c r="K122">
+        <v>18</v>
+      </c>
+      <c r="L122">
+        <v>20</v>
+      </c>
+      <c r="M122">
+        <v>12</v>
+      </c>
+      <c r="N122">
+        <v>16</v>
+      </c>
+      <c r="O122">
         <v>28</v>
       </c>
     </row>
@@ -6228,7 +6228,43 @@
         <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>13587</v>
+      </c>
+      <c r="E123">
+        <v>14027</v>
+      </c>
+      <c r="F123">
+        <v>13937</v>
+      </c>
+      <c r="G123">
+        <v>13846</v>
+      </c>
+      <c r="H123">
+        <v>13633</v>
+      </c>
+      <c r="I123">
+        <v>13461</v>
+      </c>
+      <c r="J123">
+        <v>13154</v>
+      </c>
+      <c r="K123">
+        <v>12942</v>
+      </c>
+      <c r="L123">
+        <v>12003</v>
+      </c>
+      <c r="M123">
+        <v>11645</v>
+      </c>
+      <c r="N123">
+        <v>12335</v>
+      </c>
+      <c r="O123">
+        <v>12185</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
@@ -6239,7 +6275,43 @@
         <v>0</v>
       </c>
       <c r="C124" t="s">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>59624</v>
+      </c>
+      <c r="E124">
+        <v>60771</v>
+      </c>
+      <c r="F124">
+        <v>60999</v>
+      </c>
+      <c r="G124">
+        <v>61625</v>
+      </c>
+      <c r="H124">
+        <v>62094</v>
+      </c>
+      <c r="I124">
+        <v>62076</v>
+      </c>
+      <c r="J124">
+        <v>61724</v>
+      </c>
+      <c r="K124">
+        <v>61673</v>
+      </c>
+      <c r="L124">
+        <v>59753</v>
+      </c>
+      <c r="M124">
+        <v>59525</v>
+      </c>
+      <c r="N124">
+        <v>62634</v>
+      </c>
+      <c r="O124">
+        <v>61844</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -6250,7 +6322,43 @@
         <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="D125">
+        <v>72161</v>
+      </c>
+      <c r="E125">
+        <v>73322</v>
+      </c>
+      <c r="F125">
+        <v>73216</v>
+      </c>
+      <c r="G125">
+        <v>73609</v>
+      </c>
+      <c r="H125">
+        <v>74099</v>
+      </c>
+      <c r="I125">
+        <v>73558</v>
+      </c>
+      <c r="J125">
+        <v>73338</v>
+      </c>
+      <c r="K125">
+        <v>73323</v>
+      </c>
+      <c r="L125">
+        <v>72225</v>
+      </c>
+      <c r="M125">
+        <v>72837</v>
+      </c>
+      <c r="N125">
+        <v>75325</v>
+      </c>
+      <c r="O125">
+        <v>74762</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
@@ -6261,7 +6369,43 @@
         <v>0</v>
       </c>
       <c r="C126" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="D126">
+        <v>65103</v>
+      </c>
+      <c r="E126">
+        <v>66103</v>
+      </c>
+      <c r="F126">
+        <v>66651</v>
+      </c>
+      <c r="G126">
+        <v>67340</v>
+      </c>
+      <c r="H126">
+        <v>68021</v>
+      </c>
+      <c r="I126">
+        <v>68110</v>
+      </c>
+      <c r="J126">
+        <v>68694</v>
+      </c>
+      <c r="K126">
+        <v>68967</v>
+      </c>
+      <c r="L126">
+        <v>68652</v>
+      </c>
+      <c r="M126">
+        <v>69133</v>
+      </c>
+      <c r="N126">
+        <v>71214</v>
+      </c>
+      <c r="O126">
+        <v>70195</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -6272,7 +6416,43 @@
         <v>0</v>
       </c>
       <c r="C127" t="s">
-        <v>33</v>
+        <v>6</v>
+      </c>
+      <c r="D127">
+        <v>46900</v>
+      </c>
+      <c r="E127">
+        <v>47527</v>
+      </c>
+      <c r="F127">
+        <v>48025</v>
+      </c>
+      <c r="G127">
+        <v>48636</v>
+      </c>
+      <c r="H127">
+        <v>49035</v>
+      </c>
+      <c r="I127">
+        <v>49061</v>
+      </c>
+      <c r="J127">
+        <v>49203</v>
+      </c>
+      <c r="K127">
+        <v>49311</v>
+      </c>
+      <c r="L127">
+        <v>49166</v>
+      </c>
+      <c r="M127">
+        <v>49727</v>
+      </c>
+      <c r="N127">
+        <v>51081</v>
+      </c>
+      <c r="O127">
+        <v>50600</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
@@ -6283,10 +6463,46 @@
         <v>0</v>
       </c>
       <c r="C128" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D128">
+        <v>36033</v>
+      </c>
+      <c r="E128">
+        <v>36607</v>
+      </c>
+      <c r="F128">
+        <v>36794</v>
+      </c>
+      <c r="G128">
+        <v>37094</v>
+      </c>
+      <c r="H128">
+        <v>37222</v>
+      </c>
+      <c r="I128">
+        <v>36977</v>
+      </c>
+      <c r="J128">
+        <v>36991</v>
+      </c>
+      <c r="K128">
+        <v>37107</v>
+      </c>
+      <c r="L128">
+        <v>36984</v>
+      </c>
+      <c r="M128">
+        <v>37381</v>
+      </c>
+      <c r="N128">
+        <v>38280</v>
+      </c>
+      <c r="O128">
+        <v>37998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2013</v>
       </c>
@@ -6294,10 +6510,46 @@
         <v>0</v>
       </c>
       <c r="C129" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D129">
+        <v>30553</v>
+      </c>
+      <c r="E129">
+        <v>31077</v>
+      </c>
+      <c r="F129">
+        <v>31426</v>
+      </c>
+      <c r="G129">
+        <v>31691</v>
+      </c>
+      <c r="H129">
+        <v>31918</v>
+      </c>
+      <c r="I129">
+        <v>31824</v>
+      </c>
+      <c r="J129">
+        <v>31978</v>
+      </c>
+      <c r="K129">
+        <v>31957</v>
+      </c>
+      <c r="L129">
+        <v>31890</v>
+      </c>
+      <c r="M129">
+        <v>32250</v>
+      </c>
+      <c r="N129">
+        <v>32871</v>
+      </c>
+      <c r="O129">
+        <v>32686</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2013</v>
       </c>
@@ -6305,10 +6557,46 @@
         <v>0</v>
       </c>
       <c r="C130" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D130">
+        <v>24317</v>
+      </c>
+      <c r="E130">
+        <v>24748</v>
+      </c>
+      <c r="F130">
+        <v>24961</v>
+      </c>
+      <c r="G130">
+        <v>25159</v>
+      </c>
+      <c r="H130">
+        <v>25369</v>
+      </c>
+      <c r="I130">
+        <v>25397</v>
+      </c>
+      <c r="J130">
+        <v>25520</v>
+      </c>
+      <c r="K130">
+        <v>25645</v>
+      </c>
+      <c r="L130">
+        <v>25814</v>
+      </c>
+      <c r="M130">
+        <v>26043</v>
+      </c>
+      <c r="N130">
+        <v>26564</v>
+      </c>
+      <c r="O130">
+        <v>26377</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2013</v>
       </c>
@@ -6316,10 +6604,46 @@
         <v>0</v>
       </c>
       <c r="C131" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D131">
+        <v>16844</v>
+      </c>
+      <c r="E131">
+        <v>17190</v>
+      </c>
+      <c r="F131">
+        <v>17672</v>
+      </c>
+      <c r="G131">
+        <v>18469</v>
+      </c>
+      <c r="H131">
+        <v>17982</v>
+      </c>
+      <c r="I131">
+        <v>18008</v>
+      </c>
+      <c r="J131">
+        <v>18157</v>
+      </c>
+      <c r="K131">
+        <v>18505</v>
+      </c>
+      <c r="L131">
+        <v>18576</v>
+      </c>
+      <c r="M131">
+        <v>18824</v>
+      </c>
+      <c r="N131">
+        <v>19415</v>
+      </c>
+      <c r="O131">
+        <v>19666</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2013</v>
       </c>
@@ -6327,10 +6651,46 @@
         <v>0</v>
       </c>
       <c r="C132" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D132">
+        <v>6276</v>
+      </c>
+      <c r="E132">
+        <v>6358</v>
+      </c>
+      <c r="F132">
+        <v>6380</v>
+      </c>
+      <c r="G132">
+        <v>6425</v>
+      </c>
+      <c r="H132">
+        <v>6422</v>
+      </c>
+      <c r="I132">
+        <v>6440</v>
+      </c>
+      <c r="J132">
+        <v>6498</v>
+      </c>
+      <c r="K132">
+        <v>6573</v>
+      </c>
+      <c r="L132">
+        <v>6624</v>
+      </c>
+      <c r="M132">
+        <v>6699</v>
+      </c>
+      <c r="N132">
+        <v>6711</v>
+      </c>
+      <c r="O132">
+        <v>6735</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2013</v>
       </c>
@@ -6338,10 +6698,46 @@
         <v>0</v>
       </c>
       <c r="C133" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D133">
+        <v>3630</v>
+      </c>
+      <c r="E133">
+        <v>3665</v>
+      </c>
+      <c r="F133">
+        <v>3678</v>
+      </c>
+      <c r="G133">
+        <v>3653</v>
+      </c>
+      <c r="H133">
+        <v>3642</v>
+      </c>
+      <c r="I133">
+        <v>3600</v>
+      </c>
+      <c r="J133">
+        <v>3635</v>
+      </c>
+      <c r="K133">
+        <v>3800</v>
+      </c>
+      <c r="L133">
+        <v>3846</v>
+      </c>
+      <c r="M133">
+        <v>3903</v>
+      </c>
+      <c r="N133">
+        <v>3923</v>
+      </c>
+      <c r="O133">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2013</v>
       </c>
@@ -6349,10 +6745,46 @@
         <v>26</v>
       </c>
       <c r="C134" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D134">
+        <v>12</v>
+      </c>
+      <c r="E134">
+        <v>12</v>
+      </c>
+      <c r="F134">
+        <v>9</v>
+      </c>
+      <c r="G134">
+        <v>15</v>
+      </c>
+      <c r="H134">
+        <v>12</v>
+      </c>
+      <c r="I134">
+        <v>6</v>
+      </c>
+      <c r="J134">
+        <v>5</v>
+      </c>
+      <c r="K134">
+        <v>7</v>
+      </c>
+      <c r="L134">
+        <v>8</v>
+      </c>
+      <c r="M134">
+        <v>9</v>
+      </c>
+      <c r="N134">
+        <v>8</v>
+      </c>
+      <c r="O134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2013</v>
       </c>
@@ -6360,10 +6792,46 @@
         <v>26</v>
       </c>
       <c r="C135" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>6548</v>
+      </c>
+      <c r="E135">
+        <v>6729</v>
+      </c>
+      <c r="F135">
+        <v>6592</v>
+      </c>
+      <c r="G135">
+        <v>6495</v>
+      </c>
+      <c r="H135">
+        <v>6459</v>
+      </c>
+      <c r="I135">
+        <v>6637</v>
+      </c>
+      <c r="J135">
+        <v>6472</v>
+      </c>
+      <c r="K135">
+        <v>6352</v>
+      </c>
+      <c r="L135">
+        <v>5909</v>
+      </c>
+      <c r="M135">
+        <v>5740</v>
+      </c>
+      <c r="N135">
+        <v>5735</v>
+      </c>
+      <c r="O135">
+        <v>5792</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2013</v>
       </c>
@@ -6371,10 +6839,46 @@
         <v>26</v>
       </c>
       <c r="C136" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D136">
+        <v>38568</v>
+      </c>
+      <c r="E136">
+        <v>39208</v>
+      </c>
+      <c r="F136">
+        <v>38985</v>
+      </c>
+      <c r="G136">
+        <v>39217</v>
+      </c>
+      <c r="H136">
+        <v>39832</v>
+      </c>
+      <c r="I136">
+        <v>40489</v>
+      </c>
+      <c r="J136">
+        <v>40351</v>
+      </c>
+      <c r="K136">
+        <v>40522</v>
+      </c>
+      <c r="L136">
+        <v>39604</v>
+      </c>
+      <c r="M136">
+        <v>39693</v>
+      </c>
+      <c r="N136">
+        <v>39978</v>
+      </c>
+      <c r="O136">
+        <v>39389</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2013</v>
       </c>
@@ -6382,10 +6886,46 @@
         <v>26</v>
       </c>
       <c r="C137" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D137">
+        <v>53360</v>
+      </c>
+      <c r="E137">
+        <v>53961</v>
+      </c>
+      <c r="F137">
+        <v>53509</v>
+      </c>
+      <c r="G137">
+        <v>53647</v>
+      </c>
+      <c r="H137">
+        <v>53936</v>
+      </c>
+      <c r="I137">
+        <v>54434</v>
+      </c>
+      <c r="J137">
+        <v>54404</v>
+      </c>
+      <c r="K137">
+        <v>54509</v>
+      </c>
+      <c r="L137">
+        <v>53941</v>
+      </c>
+      <c r="M137">
+        <v>54027</v>
+      </c>
+      <c r="N137">
+        <v>54519</v>
+      </c>
+      <c r="O137">
+        <v>54206</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2013</v>
       </c>
@@ -6393,10 +6933,46 @@
         <v>26</v>
       </c>
       <c r="C138" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D138">
+        <v>49518</v>
+      </c>
+      <c r="E138">
+        <v>50333</v>
+      </c>
+      <c r="F138">
+        <v>50519</v>
+      </c>
+      <c r="G138">
+        <v>50826</v>
+      </c>
+      <c r="H138">
+        <v>51497</v>
+      </c>
+      <c r="I138">
+        <v>52012</v>
+      </c>
+      <c r="J138">
+        <v>52204</v>
+      </c>
+      <c r="K138">
+        <v>52666</v>
+      </c>
+      <c r="L138">
+        <v>52535</v>
+      </c>
+      <c r="M138">
+        <v>53053</v>
+      </c>
+      <c r="N138">
+        <v>53443</v>
+      </c>
+      <c r="O138">
+        <v>53214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2013</v>
       </c>
@@ -6404,10 +6980,46 @@
         <v>26</v>
       </c>
       <c r="C139" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D139">
+        <v>36597</v>
+      </c>
+      <c r="E139">
+        <v>37144</v>
+      </c>
+      <c r="F139">
+        <v>37234</v>
+      </c>
+      <c r="G139">
+        <v>37482</v>
+      </c>
+      <c r="H139">
+        <v>37821</v>
+      </c>
+      <c r="I139">
+        <v>37971</v>
+      </c>
+      <c r="J139">
+        <v>38063</v>
+      </c>
+      <c r="K139">
+        <v>38418</v>
+      </c>
+      <c r="L139">
+        <v>38406</v>
+      </c>
+      <c r="M139">
+        <v>38788</v>
+      </c>
+      <c r="N139">
+        <v>39038</v>
+      </c>
+      <c r="O139">
+        <v>39023</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2013</v>
       </c>
@@ -6415,10 +7027,46 @@
         <v>26</v>
       </c>
       <c r="C140" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D140">
+        <v>30929</v>
+      </c>
+      <c r="E140">
+        <v>31296</v>
+      </c>
+      <c r="F140">
+        <v>31254</v>
+      </c>
+      <c r="G140">
+        <v>31414</v>
+      </c>
+      <c r="H140">
+        <v>31417</v>
+      </c>
+      <c r="I140">
+        <v>31447</v>
+      </c>
+      <c r="J140">
+        <v>31557</v>
+      </c>
+      <c r="K140">
+        <v>31549</v>
+      </c>
+      <c r="L140">
+        <v>31463</v>
+      </c>
+      <c r="M140">
+        <v>31658</v>
+      </c>
+      <c r="N140">
+        <v>31884</v>
+      </c>
+      <c r="O140">
+        <v>31696</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2013</v>
       </c>
@@ -6426,10 +7074,46 @@
         <v>26</v>
       </c>
       <c r="C141" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D141">
+        <v>25888</v>
+      </c>
+      <c r="E141">
+        <v>26206</v>
+      </c>
+      <c r="F141">
+        <v>26477</v>
+      </c>
+      <c r="G141">
+        <v>26709</v>
+      </c>
+      <c r="H141">
+        <v>26937</v>
+      </c>
+      <c r="I141">
+        <v>27068</v>
+      </c>
+      <c r="J141">
+        <v>27146</v>
+      </c>
+      <c r="K141">
+        <v>27310</v>
+      </c>
+      <c r="L141">
+        <v>27497</v>
+      </c>
+      <c r="M141">
+        <v>27793</v>
+      </c>
+      <c r="N141">
+        <v>27860</v>
+      </c>
+      <c r="O141">
+        <v>27869</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2013</v>
       </c>
@@ -6437,10 +7121,46 @@
         <v>26</v>
       </c>
       <c r="C142" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D142">
+        <v>18699</v>
+      </c>
+      <c r="E142">
+        <v>19056</v>
+      </c>
+      <c r="F142">
+        <v>19246</v>
+      </c>
+      <c r="G142">
+        <v>19535</v>
+      </c>
+      <c r="H142">
+        <v>19693</v>
+      </c>
+      <c r="I142">
+        <v>19870</v>
+      </c>
+      <c r="J142">
+        <v>20066</v>
+      </c>
+      <c r="K142">
+        <v>20315</v>
+      </c>
+      <c r="L142">
+        <v>20429</v>
+      </c>
+      <c r="M142">
+        <v>20726</v>
+      </c>
+      <c r="N142">
+        <v>20876</v>
+      </c>
+      <c r="O142">
+        <v>20953</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2013</v>
       </c>
@@ -6448,10 +7168,46 @@
         <v>26</v>
       </c>
       <c r="C143" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D143">
+        <v>10968</v>
+      </c>
+      <c r="E143">
+        <v>11190</v>
+      </c>
+      <c r="F143">
+        <v>11325</v>
+      </c>
+      <c r="G143">
+        <v>11516</v>
+      </c>
+      <c r="H143">
+        <v>11605</v>
+      </c>
+      <c r="I143">
+        <v>11606</v>
+      </c>
+      <c r="J143">
+        <v>11654</v>
+      </c>
+      <c r="K143">
+        <v>11858</v>
+      </c>
+      <c r="L143">
+        <v>12115</v>
+      </c>
+      <c r="M143">
+        <v>12395</v>
+      </c>
+      <c r="N143">
+        <v>12558</v>
+      </c>
+      <c r="O143">
+        <v>12789</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2013</v>
       </c>
@@ -6459,7 +7215,43 @@
         <v>26</v>
       </c>
       <c r="C144" t="s">
-        <v>38</v>
+        <v>11</v>
+      </c>
+      <c r="D144">
+        <v>3644</v>
+      </c>
+      <c r="E144">
+        <v>3686</v>
+      </c>
+      <c r="F144">
+        <v>3742</v>
+      </c>
+      <c r="G144">
+        <v>3750</v>
+      </c>
+      <c r="H144">
+        <v>3821</v>
+      </c>
+      <c r="I144">
+        <v>3842</v>
+      </c>
+      <c r="J144">
+        <v>3903</v>
+      </c>
+      <c r="K144">
+        <v>3979</v>
+      </c>
+      <c r="L144">
+        <v>4037</v>
+      </c>
+      <c r="M144">
+        <v>4150</v>
+      </c>
+      <c r="N144">
+        <v>4217</v>
+      </c>
+      <c r="O144">
+        <v>4235</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
@@ -6470,7 +7262,43 @@
         <v>26</v>
       </c>
       <c r="C145" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="D145">
+        <v>1342</v>
+      </c>
+      <c r="E145">
+        <v>1367</v>
+      </c>
+      <c r="F145">
+        <v>1392</v>
+      </c>
+      <c r="G145">
+        <v>1445</v>
+      </c>
+      <c r="H145">
+        <v>1464</v>
+      </c>
+      <c r="I145">
+        <v>1478</v>
+      </c>
+      <c r="J145">
+        <v>1478</v>
+      </c>
+      <c r="K145">
+        <v>1555</v>
+      </c>
+      <c r="L145">
+        <v>1619</v>
+      </c>
+      <c r="M145">
+        <v>1656</v>
+      </c>
+      <c r="N145">
+        <v>1682</v>
+      </c>
+      <c r="O145">
+        <v>1676</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
@@ -6481,7 +7309,7 @@
         <v>0</v>
       </c>
       <c r="C146" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D146">
         <v>14</v>
@@ -6528,7 +7356,7 @@
         <v>0</v>
       </c>
       <c r="C147" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D147">
         <v>12717</v>
@@ -6575,7 +7403,7 @@
         <v>0</v>
       </c>
       <c r="C148" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D148">
         <v>53872</v>
@@ -6622,7 +7450,7 @@
         <v>0</v>
       </c>
       <c r="C149" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D149">
         <v>69688</v>
@@ -6669,7 +7497,7 @@
         <v>0</v>
       </c>
       <c r="C150" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D150">
         <v>58687</v>
@@ -6716,7 +7544,7 @@
         <v>0</v>
       </c>
       <c r="C151" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D151">
         <v>42817</v>
@@ -6763,7 +7591,7 @@
         <v>0</v>
       </c>
       <c r="C152" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D152">
         <v>33008</v>
@@ -6810,7 +7638,7 @@
         <v>0</v>
       </c>
       <c r="C153" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D153">
         <v>28532</v>
@@ -6857,7 +7685,7 @@
         <v>0</v>
       </c>
       <c r="C154" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D154">
         <v>22007</v>
@@ -6904,7 +7732,7 @@
         <v>0</v>
       </c>
       <c r="C155" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D155">
         <v>15106</v>
@@ -6951,7 +7779,7 @@
         <v>0</v>
       </c>
       <c r="C156" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D156">
         <v>5442</v>
@@ -6998,7 +7826,7 @@
         <v>0</v>
       </c>
       <c r="C157" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D157">
         <v>3155</v>
@@ -7045,7 +7873,7 @@
         <v>26</v>
       </c>
       <c r="C158" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D158">
         <v>4</v>
@@ -7092,7 +7920,7 @@
         <v>26</v>
       </c>
       <c r="C159" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D159">
         <v>6265</v>
@@ -7139,7 +7967,7 @@
         <v>26</v>
       </c>
       <c r="C160" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D160">
         <v>36071</v>
@@ -7186,7 +8014,7 @@
         <v>26</v>
       </c>
       <c r="C161" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D161">
         <v>52582</v>
@@ -7233,7 +8061,7 @@
         <v>26</v>
       </c>
       <c r="C162" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D162">
         <v>45377</v>
@@ -7280,7 +8108,7 @@
         <v>26</v>
       </c>
       <c r="C163" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D163">
         <v>34297</v>
@@ -7327,7 +8155,7 @@
         <v>26</v>
       </c>
       <c r="C164" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D164">
         <v>29334</v>
@@ -7374,7 +8202,7 @@
         <v>26</v>
       </c>
       <c r="C165" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D165">
         <v>24142</v>
@@ -7421,7 +8249,7 @@
         <v>26</v>
       </c>
       <c r="C166" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D166">
         <v>16433</v>
@@ -7468,7 +8296,7 @@
         <v>26</v>
       </c>
       <c r="C167" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D167">
         <v>9468</v>
@@ -7515,7 +8343,7 @@
         <v>26</v>
       </c>
       <c r="C168" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D168">
         <v>3030</v>
@@ -7562,7 +8390,7 @@
         <v>26</v>
       </c>
       <c r="C169" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D169">
         <v>1112</v>
@@ -7609,7 +8437,7 @@
         <v>0</v>
       </c>
       <c r="C170" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D170">
         <v>24</v>
@@ -7656,7 +8484,7 @@
         <v>0</v>
       </c>
       <c r="C171" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D171">
         <v>10179</v>
@@ -7703,7 +8531,7 @@
         <v>0</v>
       </c>
       <c r="C172" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D172">
         <v>49742</v>
@@ -7750,7 +8578,7 @@
         <v>0</v>
       </c>
       <c r="C173" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D173">
         <v>65424</v>
@@ -7797,7 +8625,7 @@
         <v>0</v>
       </c>
       <c r="C174" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D174">
         <v>52001</v>
@@ -7844,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="C175" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D175">
         <v>38940</v>
@@ -7891,7 +8719,7 @@
         <v>0</v>
       </c>
       <c r="C176" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D176">
         <v>31300</v>
@@ -7938,7 +8766,7 @@
         <v>0</v>
       </c>
       <c r="C177" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D177">
         <v>26485</v>
@@ -7985,7 +8813,7 @@
         <v>0</v>
       </c>
       <c r="C178" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D178">
         <v>20323</v>
@@ -8032,7 +8860,7 @@
         <v>0</v>
       </c>
       <c r="C179" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D179">
         <v>13324</v>
@@ -8079,7 +8907,7 @@
         <v>0</v>
       </c>
       <c r="C180" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D180">
         <v>5140</v>
@@ -8126,7 +8954,7 @@
         <v>0</v>
       </c>
       <c r="C181" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D181">
         <v>2893</v>
@@ -8173,7 +9001,7 @@
         <v>26</v>
       </c>
       <c r="C182" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D182">
         <v>16</v>
@@ -8220,7 +9048,7 @@
         <v>26</v>
       </c>
       <c r="C183" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D183">
         <v>5000</v>
@@ -8267,7 +9095,7 @@
         <v>26</v>
       </c>
       <c r="C184" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D184">
         <v>33176</v>
@@ -8314,7 +9142,7 @@
         <v>26</v>
       </c>
       <c r="C185" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D185">
         <v>49816</v>
@@ -8361,7 +9189,7 @@
         <v>26</v>
       </c>
       <c r="C186" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D186">
         <v>40444</v>
@@ -8408,7 +9236,7 @@
         <v>26</v>
       </c>
       <c r="C187" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D187">
         <v>32156</v>
@@ -8455,7 +9283,7 @@
         <v>26</v>
       </c>
       <c r="C188" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D188">
         <v>28380</v>
@@ -8502,7 +9330,7 @@
         <v>26</v>
       </c>
       <c r="C189" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D189">
         <v>22341</v>
@@ -8549,7 +9377,7 @@
         <v>26</v>
       </c>
       <c r="C190" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D190">
         <v>15051</v>
@@ -8596,7 +9424,7 @@
         <v>26</v>
       </c>
       <c r="C191" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D191">
         <v>8258</v>
@@ -8643,7 +9471,7 @@
         <v>26</v>
       </c>
       <c r="C192" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D192">
         <v>2567</v>
@@ -8690,7 +9518,7 @@
         <v>26</v>
       </c>
       <c r="C193" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D193">
         <v>991</v>
@@ -8737,7 +9565,7 @@
         <v>0</v>
       </c>
       <c r="C194" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D194">
         <v>31</v>
@@ -8784,7 +9612,7 @@
         <v>0</v>
       </c>
       <c r="C195" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D195">
         <v>10197</v>
@@ -8831,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="C196" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D196">
         <v>46494</v>
@@ -8878,7 +9706,7 @@
         <v>0</v>
       </c>
       <c r="C197" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D197">
         <v>61251</v>
@@ -8925,7 +9753,7 @@
         <v>0</v>
       </c>
       <c r="C198" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D198">
         <v>46695</v>
@@ -8972,7 +9800,7 @@
         <v>0</v>
       </c>
       <c r="C199" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D199">
         <v>35833</v>
@@ -9019,7 +9847,7 @@
         <v>0</v>
       </c>
       <c r="C200" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D200">
         <v>29971</v>
@@ -9066,7 +9894,7 @@
         <v>0</v>
       </c>
       <c r="C201" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D201">
         <v>25068</v>
@@ -9113,7 +9941,7 @@
         <v>0</v>
       </c>
       <c r="C202" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D202">
         <v>18586</v>
@@ -9160,7 +9988,7 @@
         <v>0</v>
       </c>
       <c r="C203" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D203">
         <v>11809</v>
@@ -9207,7 +10035,7 @@
         <v>0</v>
       </c>
       <c r="C204" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D204">
         <v>4853</v>
@@ -9254,7 +10082,7 @@
         <v>0</v>
       </c>
       <c r="C205" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D205">
         <v>2637</v>
@@ -9301,7 +10129,7 @@
         <v>26</v>
       </c>
       <c r="C206" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D206">
         <v>12</v>
@@ -9348,7 +10176,7 @@
         <v>26</v>
       </c>
       <c r="C207" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D207">
         <v>5346</v>
@@ -9395,7 +10223,7 @@
         <v>26</v>
       </c>
       <c r="C208" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D208">
         <v>32896</v>
@@ -9442,7 +10270,7 @@
         <v>26</v>
       </c>
       <c r="C209" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D209">
         <v>48029</v>
@@ -9489,7 +10317,7 @@
         <v>26</v>
       </c>
       <c r="C210" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D210">
         <v>37172</v>
@@ -9536,7 +10364,7 @@
         <v>26</v>
       </c>
       <c r="C211" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D211">
         <v>31148</v>
@@ -9583,7 +10411,7 @@
         <v>26</v>
       </c>
       <c r="C212" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D212">
         <v>27658</v>
@@ -9630,7 +10458,7 @@
         <v>26</v>
       </c>
       <c r="C213" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D213">
         <v>21139</v>
@@ -9677,7 +10505,7 @@
         <v>26</v>
       </c>
       <c r="C214" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D214">
         <v>13740</v>
@@ -9724,7 +10552,7 @@
         <v>26</v>
       </c>
       <c r="C215" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D215">
         <v>7277</v>
@@ -9771,7 +10599,7 @@
         <v>26</v>
       </c>
       <c r="C216" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D216">
         <v>2266</v>
@@ -9818,7 +10646,7 @@
         <v>26</v>
       </c>
       <c r="C217" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D217">
         <v>899</v>
@@ -9865,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="C218" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D218">
         <v>41</v>
@@ -9912,7 +10740,7 @@
         <v>0</v>
       </c>
       <c r="C219" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D219">
         <v>11113</v>
@@ -9959,7 +10787,7 @@
         <v>0</v>
       </c>
       <c r="C220" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D220">
         <v>45886</v>
@@ -10006,7 +10834,7 @@
         <v>0</v>
       </c>
       <c r="C221" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D221">
         <v>56706</v>
@@ -10053,7 +10881,7 @@
         <v>0</v>
       </c>
       <c r="C222" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D222">
         <v>43392</v>
@@ -10100,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="C223" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D223">
         <v>33036</v>
@@ -10147,7 +10975,7 @@
         <v>0</v>
       </c>
       <c r="C224" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D224">
         <v>28548</v>
@@ -10194,7 +11022,7 @@
         <v>0</v>
       </c>
       <c r="C225" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D225">
         <v>23558</v>
@@ -10241,7 +11069,7 @@
         <v>0</v>
       </c>
       <c r="C226" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D226">
         <v>17504</v>
@@ -10288,7 +11116,7 @@
         <v>0</v>
       </c>
       <c r="C227" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D227">
         <v>10464</v>
@@ -10335,7 +11163,7 @@
         <v>0</v>
       </c>
       <c r="C228" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D228">
         <v>4510</v>
@@ -10382,7 +11210,7 @@
         <v>0</v>
       </c>
       <c r="C229" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D229">
         <v>2453</v>
@@ -10429,7 +11257,7 @@
         <v>26</v>
       </c>
       <c r="C230" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D230">
         <v>25</v>
@@ -10476,7 +11304,7 @@
         <v>26</v>
       </c>
       <c r="C231" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D231">
         <v>5819</v>
@@ -10523,7 +11351,7 @@
         <v>26</v>
       </c>
       <c r="C232" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D232">
         <v>34284</v>
@@ -10570,7 +11398,7 @@
         <v>26</v>
       </c>
       <c r="C233" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D233">
         <v>45692</v>
@@ -10617,7 +11445,7 @@
         <v>26</v>
       </c>
       <c r="C234" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D234">
         <v>35199</v>
@@ -10664,7 +11492,7 @@
         <v>26</v>
       </c>
       <c r="C235" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D235">
         <v>29928</v>
@@ -10711,7 +11539,7 @@
         <v>26</v>
       </c>
       <c r="C236" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D236">
         <v>26595</v>
@@ -10758,7 +11586,7 @@
         <v>26</v>
       </c>
       <c r="C237" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D237">
         <v>19606</v>
@@ -10805,7 +11633,7 @@
         <v>26</v>
       </c>
       <c r="C238" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D238">
         <v>12508</v>
@@ -10852,7 +11680,7 @@
         <v>26</v>
       </c>
       <c r="C239" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D239">
         <v>6407</v>
@@ -10899,7 +11727,7 @@
         <v>26</v>
       </c>
       <c r="C240" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D240">
         <v>1993</v>
@@ -10946,7 +11774,7 @@
         <v>26</v>
       </c>
       <c r="C241" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D241">
         <v>773</v>
@@ -10993,7 +11821,7 @@
         <v>0</v>
       </c>
       <c r="C242" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D242">
         <v>36</v>
@@ -11040,7 +11868,7 @@
         <v>0</v>
       </c>
       <c r="C243" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D243">
         <v>10861</v>
@@ -11087,7 +11915,7 @@
         <v>0</v>
       </c>
       <c r="C244" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D244">
         <v>46959</v>
@@ -11134,7 +11962,7 @@
         <v>0</v>
       </c>
       <c r="C245" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D245">
         <v>54188</v>
@@ -11181,7 +12009,7 @@
         <v>0</v>
       </c>
       <c r="C246" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D246">
         <v>41162</v>
@@ -11228,7 +12056,7 @@
         <v>0</v>
       </c>
       <c r="C247" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D247">
         <v>31830</v>
@@ -11275,7 +12103,7 @@
         <v>0</v>
       </c>
       <c r="C248" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D248">
         <v>27118</v>
@@ -11322,7 +12150,7 @@
         <v>0</v>
       </c>
       <c r="C249" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D249">
         <v>21778</v>
@@ -11369,7 +12197,7 @@
         <v>0</v>
       </c>
       <c r="C250" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D250">
         <v>15525</v>
@@ -11416,7 +12244,7 @@
         <v>0</v>
       </c>
       <c r="C251" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D251">
         <v>9590</v>
@@ -11463,7 +12291,7 @@
         <v>0</v>
       </c>
       <c r="C252" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D252">
         <v>3932</v>
@@ -11510,7 +12338,7 @@
         <v>0</v>
       </c>
       <c r="C253" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D253">
         <v>2245</v>
@@ -11557,7 +12385,7 @@
         <v>26</v>
       </c>
       <c r="C254" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D254">
         <v>12</v>
@@ -11604,7 +12432,7 @@
         <v>26</v>
       </c>
       <c r="C255" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D255">
         <v>6791</v>
@@ -11651,7 +12479,7 @@
         <v>26</v>
       </c>
       <c r="C256" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D256">
         <v>36494</v>
@@ -11698,7 +12526,7 @@
         <v>26</v>
       </c>
       <c r="C257" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D257">
         <v>44566</v>
@@ -11745,7 +12573,7 @@
         <v>26</v>
       </c>
       <c r="C258" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D258">
         <v>34919</v>
@@ -11792,7 +12620,7 @@
         <v>26</v>
       </c>
       <c r="C259" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D259">
         <v>30800</v>
@@ -11839,7 +12667,7 @@
         <v>26</v>
       </c>
       <c r="C260" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D260">
         <v>25632</v>
@@ -11886,7 +12714,7 @@
         <v>26</v>
       </c>
       <c r="C261" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D261">
         <v>18194</v>
@@ -11933,7 +12761,7 @@
         <v>26</v>
       </c>
       <c r="C262" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D262">
         <v>11414</v>
@@ -11980,7 +12808,7 @@
         <v>26</v>
       </c>
       <c r="C263" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D263">
         <v>5597</v>
@@ -12027,7 +12855,7 @@
         <v>26</v>
       </c>
       <c r="C264" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D264">
         <v>1820</v>
@@ -12074,7 +12902,7 @@
         <v>26</v>
       </c>
       <c r="C265" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D265">
         <v>692</v>
@@ -12121,7 +12949,7 @@
         <v>0</v>
       </c>
       <c r="C266" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="267" spans="1:15" x14ac:dyDescent="0.25">
@@ -12132,7 +12960,7 @@
         <v>0</v>
       </c>
       <c r="C267" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268" spans="1:15" x14ac:dyDescent="0.25">
@@ -12143,7 +12971,7 @@
         <v>0</v>
       </c>
       <c r="C268" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="269" spans="1:15" x14ac:dyDescent="0.25">
@@ -12154,7 +12982,7 @@
         <v>0</v>
       </c>
       <c r="C269" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="270" spans="1:15" x14ac:dyDescent="0.25">
@@ -12165,7 +12993,7 @@
         <v>0</v>
       </c>
       <c r="C270" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.25">
@@ -12176,7 +13004,7 @@
         <v>0</v>
       </c>
       <c r="C271" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.25">
@@ -12187,7 +13015,7 @@
         <v>0</v>
       </c>
       <c r="C272" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -12198,7 +13026,7 @@
         <v>0</v>
       </c>
       <c r="C273" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -12209,7 +13037,7 @@
         <v>0</v>
       </c>
       <c r="C274" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -12220,7 +13048,7 @@
         <v>0</v>
       </c>
       <c r="C275" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -12231,7 +13059,7 @@
         <v>0</v>
       </c>
       <c r="C276" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -12242,7 +13070,7 @@
         <v>0</v>
       </c>
       <c r="C277" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -12253,7 +13081,7 @@
         <v>26</v>
       </c>
       <c r="C278" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -12264,7 +13092,7 @@
         <v>26</v>
       </c>
       <c r="C279" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -12275,7 +13103,7 @@
         <v>26</v>
       </c>
       <c r="C280" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -12286,7 +13114,7 @@
         <v>26</v>
       </c>
       <c r="C281" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -12297,7 +13125,7 @@
         <v>26</v>
       </c>
       <c r="C282" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -12308,7 +13136,7 @@
         <v>26</v>
       </c>
       <c r="C283" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -12319,7 +13147,7 @@
         <v>26</v>
       </c>
       <c r="C284" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -12330,7 +13158,7 @@
         <v>26</v>
       </c>
       <c r="C285" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -12341,7 +13169,7 @@
         <v>26</v>
       </c>
       <c r="C286" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -12352,7 +13180,7 @@
         <v>26</v>
       </c>
       <c r="C287" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -12363,7 +13191,7 @@
         <v>26</v>
       </c>
       <c r="C288" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="289" spans="1:15" x14ac:dyDescent="0.25">
@@ -12374,7 +13202,7 @@
         <v>26</v>
       </c>
       <c r="C289" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="290" spans="1:15" x14ac:dyDescent="0.25">
@@ -12385,7 +13213,7 @@
         <v>0</v>
       </c>
       <c r="C290" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D290">
         <v>18</v>
@@ -12432,7 +13260,7 @@
         <v>0</v>
       </c>
       <c r="C291" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D291">
         <v>7977</v>
@@ -12479,7 +13307,7 @@
         <v>0</v>
       </c>
       <c r="C292" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D292">
         <v>40187</v>
@@ -12526,7 +13354,7 @@
         <v>0</v>
       </c>
       <c r="C293" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D293">
         <v>42243</v>
@@ -12573,7 +13401,7 @@
         <v>0</v>
       </c>
       <c r="C294" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D294">
         <v>34051</v>
@@ -12620,7 +13448,7 @@
         <v>0</v>
       </c>
       <c r="C295" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D295">
         <v>27143</v>
@@ -12667,7 +13495,7 @@
         <v>0</v>
       </c>
       <c r="C296" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D296">
         <v>23333</v>
@@ -12714,7 +13542,7 @@
         <v>0</v>
       </c>
       <c r="C297" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D297">
         <v>17922</v>
@@ -12761,7 +13589,7 @@
         <v>0</v>
       </c>
       <c r="C298" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D298">
         <v>11935</v>
@@ -12808,7 +13636,7 @@
         <v>0</v>
       </c>
       <c r="C299" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D299">
         <v>7593</v>
@@ -12855,7 +13683,7 @@
         <v>0</v>
       </c>
       <c r="C300" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D300">
         <v>3122</v>
@@ -12902,7 +13730,7 @@
         <v>0</v>
       </c>
       <c r="C301" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D301">
         <v>1979</v>
@@ -12949,7 +13777,7 @@
         <v>26</v>
       </c>
       <c r="C302" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D302">
         <v>8</v>
@@ -12996,7 +13824,7 @@
         <v>26</v>
       </c>
       <c r="C303" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D303">
         <v>5091</v>
@@ -13043,7 +13871,7 @@
         <v>26</v>
       </c>
       <c r="C304" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D304">
         <v>32079</v>
@@ -13090,7 +13918,7 @@
         <v>26</v>
       </c>
       <c r="C305" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D305">
         <v>35940</v>
@@ -13137,7 +13965,7 @@
         <v>26</v>
       </c>
       <c r="C306" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D306">
         <v>30311</v>
@@ -13184,7 +14012,7 @@
         <v>26</v>
       </c>
       <c r="C307" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D307">
         <v>27730</v>
@@ -13231,7 +14059,7 @@
         <v>26</v>
       </c>
       <c r="C308" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D308">
         <v>22192</v>
@@ -13278,7 +14106,7 @@
         <v>26</v>
       </c>
       <c r="C309" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D309">
         <v>14956</v>
@@ -13325,7 +14153,7 @@
         <v>26</v>
       </c>
       <c r="C310" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D310">
         <v>8645</v>
@@ -13372,7 +14200,7 @@
         <v>26</v>
       </c>
       <c r="C311" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D311">
         <v>4078</v>
@@ -13419,7 +14247,7 @@
         <v>26</v>
       </c>
       <c r="C312" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D312">
         <v>1334</v>
@@ -13466,7 +14294,7 @@
         <v>26</v>
       </c>
       <c r="C313" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D313">
         <v>542</v>

</xml_diff>